<commit_message>
Update for admission 3rd test case. fix xpaths.
</commit_message>
<xml_diff>
--- a/resources/admissionForNewPatient.xlsx
+++ b/resources/admissionForNewPatient.xlsx
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15"/>
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" ht="30">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" ht="75">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" ht="45">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>